<commit_message>
uloha_01: Všechno kromě úkolu 3 (snad)
</commit_message>
<xml_diff>
--- a/uloha_01/data_01/data_01.xlsx
+++ b/uloha_01/data_01/data_01.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="volne" sheetId="1" r:id="rId1"/>
-    <sheet name="prevodni_tabulka" sheetId="4" r:id="rId2"/>
-    <sheet name="zesilovac" sheetId="2" r:id="rId3"/>
-    <sheet name="q-spinani" sheetId="3" r:id="rId4"/>
+    <sheet name="zesilovac" sheetId="2" r:id="rId2"/>
+    <sheet name="q-spinani" sheetId="3" r:id="rId3"/>
+    <sheet name="prevodni_tabulka" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -131,9 +131,6 @@
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -143,6 +140,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normální" xfId="0" builtinId="0"/>
@@ -351,14 +351,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="10"/>
+      <c r="C1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1"/>
+      <c r="D1" s="10"/>
       <c r="F1" t="s">
         <v>2</v>
       </c>
@@ -402,13 +402,13 @@
       <c r="D3">
         <v>0</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="1">
         <v>220</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -545,13 +545,13 @@
       <c r="D10">
         <v>186</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="2">
         <v>550</v>
       </c>
       <c r="F10">
         <v>175</v>
       </c>
-      <c r="G10" s="4" t="s">
+      <c r="G10" s="3" t="s">
         <v>7</v>
       </c>
     </row>
@@ -608,13 +608,13 @@
       <c r="D13">
         <v>318</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="4">
         <v>700</v>
       </c>
       <c r="F13">
         <v>348</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="G13" s="4" t="s">
         <v>8</v>
       </c>
     </row>
@@ -634,477 +634,6 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B57"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="10">
-        <v>200</v>
-      </c>
-      <c r="B2" s="10">
-        <v>369</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="10">
-        <v>210</v>
-      </c>
-      <c r="B3" s="10">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="10">
-        <v>220</v>
-      </c>
-      <c r="B4" s="10">
-        <v>371</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="10">
-        <v>230</v>
-      </c>
-      <c r="B5" s="10">
-        <v>373</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="10">
-        <v>240</v>
-      </c>
-      <c r="B6" s="10">
-        <v>374</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="10">
-        <v>250</v>
-      </c>
-      <c r="B7" s="10">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>260</v>
-      </c>
-      <c r="B8" s="10">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>270</v>
-      </c>
-      <c r="B9" s="10">
-        <v>381</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>280</v>
-      </c>
-      <c r="B10" s="10">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>290</v>
-      </c>
-      <c r="B11" s="10">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>300</v>
-      </c>
-      <c r="B12" s="10">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>310</v>
-      </c>
-      <c r="B13" s="10">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>320</v>
-      </c>
-      <c r="B14" s="10">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>330</v>
-      </c>
-      <c r="B15" s="10">
-        <v>402</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>340</v>
-      </c>
-      <c r="B16" s="10">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>350</v>
-      </c>
-      <c r="B17" s="10">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>360</v>
-      </c>
-      <c r="B18" s="10">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>370</v>
-      </c>
-      <c r="B19" s="10">
-        <v>421</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>380</v>
-      </c>
-      <c r="B20" s="10">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>390</v>
-      </c>
-      <c r="B21" s="10">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>400</v>
-      </c>
-      <c r="B22" s="10">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <v>410</v>
-      </c>
-      <c r="B23" s="10">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <v>420</v>
-      </c>
-      <c r="B24" s="10">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25">
-        <v>430</v>
-      </c>
-      <c r="B25" s="10">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26">
-        <v>440</v>
-      </c>
-      <c r="B26" s="10">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27">
-        <v>450</v>
-      </c>
-      <c r="B27" s="10">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28">
-        <v>460</v>
-      </c>
-      <c r="B28" s="10">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29">
-        <v>470</v>
-      </c>
-      <c r="B29">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30">
-        <v>480</v>
-      </c>
-      <c r="B30">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31">
-        <v>490</v>
-      </c>
-      <c r="B31">
-        <v>506</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32">
-        <v>500</v>
-      </c>
-      <c r="B32">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33">
-        <v>510</v>
-      </c>
-      <c r="B33">
-        <v>524</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34">
-        <v>520</v>
-      </c>
-      <c r="B34">
-        <v>534</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35">
-        <v>530</v>
-      </c>
-      <c r="B35">
-        <v>543</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36">
-        <v>540</v>
-      </c>
-      <c r="B36">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37">
-        <v>550</v>
-      </c>
-      <c r="B37">
-        <v>563</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38">
-        <v>560</v>
-      </c>
-      <c r="B38">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A39">
-        <v>570</v>
-      </c>
-      <c r="B39">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A40">
-        <v>580</v>
-      </c>
-      <c r="B40">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A41">
-        <v>590</v>
-      </c>
-      <c r="B41">
-        <v>607</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A42">
-        <v>600</v>
-      </c>
-      <c r="B42">
-        <v>619</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A43">
-        <v>610</v>
-      </c>
-      <c r="B43">
-        <v>631</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A44">
-        <v>620</v>
-      </c>
-      <c r="B44">
-        <v>643</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A45">
-        <v>630</v>
-      </c>
-      <c r="B45">
-        <v>655</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A46">
-        <v>640</v>
-      </c>
-      <c r="B46">
-        <v>668</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A47">
-        <v>650</v>
-      </c>
-      <c r="B47">
-        <v>681</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A48">
-        <v>660</v>
-      </c>
-      <c r="B48">
-        <v>694</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A49">
-        <v>670</v>
-      </c>
-      <c r="B49">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A50">
-        <v>680</v>
-      </c>
-      <c r="B50">
-        <v>720</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A51">
-        <v>690</v>
-      </c>
-      <c r="B51">
-        <v>735</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A52">
-        <v>700</v>
-      </c>
-      <c r="B52">
-        <v>750</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A53">
-        <v>710</v>
-      </c>
-      <c r="B53">
-        <v>765</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A54">
-        <v>720</v>
-      </c>
-      <c r="B54">
-        <v>780</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A55">
-        <v>730</v>
-      </c>
-      <c r="B55">
-        <v>795</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A56">
-        <v>740</v>
-      </c>
-      <c r="B56">
-        <v>810</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A57">
-        <v>750</v>
-      </c>
-      <c r="B57">
-        <v>825</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -1127,7 +656,7 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="6">
+      <c r="A3" s="5">
         <v>220</v>
       </c>
       <c r="B3">
@@ -1183,7 +712,7 @@
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="7">
+      <c r="A10" s="6">
         <v>550</v>
       </c>
       <c r="B10">
@@ -1207,7 +736,7 @@
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="7">
+      <c r="A13" s="6">
         <v>700</v>
       </c>
       <c r="B13">
@@ -1224,7 +753,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
@@ -1254,13 +783,13 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="9">
+      <c r="A3" s="8">
         <v>23.8</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="8">
         <v>20</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="8" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1313,13 +842,13 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="8">
+      <c r="A10" s="7">
         <v>25.4</v>
       </c>
-      <c r="B10" s="8">
+      <c r="B10" s="7">
         <v>26</v>
       </c>
-      <c r="C10" s="8"/>
+      <c r="C10" s="7"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11">
@@ -1337,4 +866,475 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Běžné"&amp;12Stránka &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B57"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="9">
+        <v>200</v>
+      </c>
+      <c r="B2" s="9">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="9">
+        <v>210</v>
+      </c>
+      <c r="B3" s="9">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="9">
+        <v>220</v>
+      </c>
+      <c r="B4" s="9">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="9">
+        <v>230</v>
+      </c>
+      <c r="B5" s="9">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="9">
+        <v>240</v>
+      </c>
+      <c r="B6" s="9">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="9">
+        <v>250</v>
+      </c>
+      <c r="B7" s="9">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>260</v>
+      </c>
+      <c r="B8" s="9">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>270</v>
+      </c>
+      <c r="B9" s="9">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>280</v>
+      </c>
+      <c r="B10" s="9">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>290</v>
+      </c>
+      <c r="B11" s="9">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>300</v>
+      </c>
+      <c r="B12" s="9">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>310</v>
+      </c>
+      <c r="B13" s="9">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>320</v>
+      </c>
+      <c r="B14" s="9">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>330</v>
+      </c>
+      <c r="B15" s="9">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>340</v>
+      </c>
+      <c r="B16" s="9">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>350</v>
+      </c>
+      <c r="B17" s="9">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>360</v>
+      </c>
+      <c r="B18" s="9">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>370</v>
+      </c>
+      <c r="B19" s="9">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>380</v>
+      </c>
+      <c r="B20" s="9">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>390</v>
+      </c>
+      <c r="B21" s="9">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>400</v>
+      </c>
+      <c r="B22" s="9">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>410</v>
+      </c>
+      <c r="B23" s="9">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>420</v>
+      </c>
+      <c r="B24" s="9">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>430</v>
+      </c>
+      <c r="B25" s="9">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>440</v>
+      </c>
+      <c r="B26" s="9">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>450</v>
+      </c>
+      <c r="B27" s="9">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>460</v>
+      </c>
+      <c r="B28" s="9">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>470</v>
+      </c>
+      <c r="B29">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>480</v>
+      </c>
+      <c r="B30">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>490</v>
+      </c>
+      <c r="B31">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>500</v>
+      </c>
+      <c r="B32">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>510</v>
+      </c>
+      <c r="B33">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>520</v>
+      </c>
+      <c r="B34">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>530</v>
+      </c>
+      <c r="B35">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>540</v>
+      </c>
+      <c r="B36">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>550</v>
+      </c>
+      <c r="B37">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>560</v>
+      </c>
+      <c r="B38">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>570</v>
+      </c>
+      <c r="B39">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>580</v>
+      </c>
+      <c r="B40">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>590</v>
+      </c>
+      <c r="B41">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>600</v>
+      </c>
+      <c r="B42">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>610</v>
+      </c>
+      <c r="B43">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>620</v>
+      </c>
+      <c r="B44">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>630</v>
+      </c>
+      <c r="B45">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>640</v>
+      </c>
+      <c r="B46">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>650</v>
+      </c>
+      <c r="B47">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>660</v>
+      </c>
+      <c r="B48">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>670</v>
+      </c>
+      <c r="B49">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>680</v>
+      </c>
+      <c r="B50">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>690</v>
+      </c>
+      <c r="B51">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>700</v>
+      </c>
+      <c r="B52">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>710</v>
+      </c>
+      <c r="B53">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>720</v>
+      </c>
+      <c r="B54">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>730</v>
+      </c>
+      <c r="B55">
+        <v>795</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>740</v>
+      </c>
+      <c r="B56">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>750</v>
+      </c>
+      <c r="B57">
+        <v>825</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
uloha_01: Úprava PDF se zadáním - přidání výpočtů
</commit_message>
<xml_diff>
--- a/uloha_01/data_01/data_01.xlsx
+++ b/uloha_01/data_01/data_01.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="volne" sheetId="1" r:id="rId1"/>
@@ -636,7 +636,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -870,9 +870,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B57"/>
+  <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A47" workbookViewId="0">
       <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
@@ -1134,7 +1134,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>510</v>
       </c>
@@ -1142,7 +1142,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>520</v>
       </c>
@@ -1150,7 +1150,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>530</v>
       </c>
@@ -1158,7 +1158,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>540</v>
       </c>
@@ -1166,15 +1166,18 @@
         <v>553</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>550</v>
       </c>
       <c r="B37">
         <v>563</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="E37">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>560</v>
       </c>
@@ -1182,7 +1185,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>570</v>
       </c>
@@ -1190,7 +1193,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>580</v>
       </c>
@@ -1198,7 +1201,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>590</v>
       </c>
@@ -1206,7 +1209,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>600</v>
       </c>
@@ -1214,7 +1217,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>610</v>
       </c>
@@ -1222,7 +1225,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>620</v>
       </c>
@@ -1230,7 +1233,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>630</v>
       </c>
@@ -1238,7 +1241,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>640</v>
       </c>
@@ -1246,7 +1249,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>650</v>
       </c>
@@ -1254,7 +1257,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>660</v>
       </c>

</xml_diff>